<commit_message>
added all runs of the resnet-50 and 101 models
</commit_message>
<xml_diff>
--- a/Model_Summary.xlsx
+++ b/Model_Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soumi\workspace\winter2024\enel645\Assignments &amp; Project\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A0C516-FAA4-46FE-A23B-D76C61253E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F7798F-F19B-44BB-87B3-A1ECBD180231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
   <si>
     <t xml:space="preserve">MODEL </t>
   </si>
@@ -216,12 +216,6 @@
     <t>bestmodel_44_rn50</t>
   </si>
   <si>
-    <t xml:space="preserve">food_4_rn101.slurm / </t>
-  </si>
-  <si>
-    <t xml:space="preserve">food_44_rn101.slurm / </t>
-  </si>
-  <si>
     <t>bestmodel_4_rn101</t>
   </si>
   <si>
@@ -232,6 +226,12 @@
   </si>
   <si>
     <t>food_44_rn50.slurm / 20663</t>
+  </si>
+  <si>
+    <t>food_4_rn101.slurm / 24437</t>
+  </si>
+  <si>
+    <t>food_44_rn101.slurm / 24438</t>
   </si>
 </sst>
 </file>
@@ -254,7 +254,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,12 +285,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="28">
     <border>
@@ -673,38 +667,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -723,9 +699,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -741,19 +714,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -795,6 +759,57 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -817,6 +832,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -828,12 +870,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -843,79 +879,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1200,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1227,159 +1200,159 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:17" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="54" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="41" t="s">
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="42"/>
-      <c r="P2" s="43"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="50"/>
     </row>
     <row r="3" spans="2:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="50"/>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="66"/>
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="37" t="s">
+      <c r="J3" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="39" t="s">
+      <c r="M3" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="44"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="46"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="53"/>
     </row>
     <row r="4" spans="2:17" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="19">
         <v>1E-4</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="13">
         <v>32</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="13">
         <v>15</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="13">
         <v>3</v>
       </c>
-      <c r="H4" s="20">
+      <c r="H4" s="13">
         <v>0.1</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="I4" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="22">
+      <c r="J4" s="15">
         <v>0.87939999999999996</v>
       </c>
-      <c r="K4" s="20">
+      <c r="K4" s="13">
         <v>0.79879999999999995</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="24" t="s">
+      <c r="M4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="N4" s="29" t="s">
+      <c r="N4" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="47" t="s">
+      <c r="O4" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="P4" s="48"/>
+      <c r="P4" s="55"/>
       <c r="Q4" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="2:17" ht="87" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="52"/>
-      <c r="C5" s="33">
+      <c r="B5" s="46"/>
+      <c r="C5" s="23">
         <v>1E-4</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="5">
         <v>32</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="5">
         <v>15</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="5">
         <v>3</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="5">
         <v>0.1</v>
       </c>
-      <c r="I5" s="34" t="s">
+      <c r="I5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="30">
+      <c r="J5" s="20">
         <v>0.91610000000000003</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="5">
         <v>0.83069999999999999</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="M5" s="25" t="s">
+      <c r="M5" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="N5" s="60" t="s">
+      <c r="N5" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="61" t="s">
+      <c r="O5" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="P5" s="62" t="s">
+      <c r="P5" s="60" t="s">
         <v>23</v>
       </c>
       <c r="Q5" s="1">
@@ -1388,385 +1361,393 @@
       </c>
     </row>
     <row r="6" spans="2:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="B6" s="52"/>
-      <c r="C6" s="33">
+      <c r="B6" s="46"/>
+      <c r="C6" s="23">
         <v>1E-3</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="5">
         <v>32</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="5">
         <v>15</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="5">
         <v>3</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="5">
         <v>0.1</v>
       </c>
-      <c r="I6" s="34" t="s">
+      <c r="I6" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="30">
+      <c r="J6" s="20">
         <v>0.86439999999999995</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="5">
         <v>0.78039999999999998</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="25" t="s">
+      <c r="M6" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="N6" s="60"/>
-      <c r="O6" s="61"/>
-      <c r="P6" s="62"/>
+      <c r="N6" s="56"/>
+      <c r="O6" s="58"/>
+      <c r="P6" s="60"/>
       <c r="Q6" s="1">
         <f t="shared" ref="Q6:Q22" si="0">J6-K6</f>
         <v>8.3999999999999964E-2</v>
       </c>
     </row>
     <row r="7" spans="2:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="B7" s="52"/>
-      <c r="C7" s="33">
+      <c r="B7" s="46"/>
+      <c r="C7" s="23">
         <v>0.01</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="5">
         <v>32</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="5">
         <v>15</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="5">
         <v>3</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="5">
         <v>0.1</v>
       </c>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="30">
+      <c r="J7" s="20">
         <v>0.30009999999999998</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="5">
         <v>0.2893</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="L7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="M7" s="25" t="s">
+      <c r="M7" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="N7" s="60"/>
-      <c r="O7" s="61"/>
-      <c r="P7" s="62"/>
+      <c r="N7" s="56"/>
+      <c r="O7" s="58"/>
+      <c r="P7" s="60"/>
       <c r="Q7" s="1">
         <f t="shared" si="0"/>
         <v>1.0799999999999976E-2</v>
       </c>
     </row>
     <row r="8" spans="2:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="B8" s="52"/>
-      <c r="C8" s="40">
+      <c r="B8" s="46"/>
+      <c r="C8" s="30">
         <v>1E-4</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="5">
         <v>32</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="5">
         <v>15</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="5">
         <v>3</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="5">
         <v>0.1</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="30">
+      <c r="J8" s="20">
         <v>0.91359999999999997</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="5">
         <v>0.82730000000000004</v>
       </c>
-      <c r="L8" s="11" t="s">
+      <c r="L8" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M8" s="25" t="s">
+      <c r="M8" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="N8" s="60"/>
-      <c r="O8" s="61"/>
-      <c r="P8" s="62"/>
+      <c r="N8" s="56"/>
+      <c r="O8" s="58"/>
+      <c r="P8" s="60"/>
       <c r="Q8" s="1">
         <f t="shared" si="0"/>
         <v>8.6299999999999932E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:17" s="79" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="B9" s="52"/>
-      <c r="C9" s="69">
+    <row r="9" spans="2:17" s="43" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B9" s="46"/>
+      <c r="C9" s="33">
         <v>1E-4</v>
       </c>
-      <c r="D9" s="70">
+      <c r="D9" s="34">
         <v>32</v>
       </c>
-      <c r="E9" s="70">
+      <c r="E9" s="34">
         <v>15</v>
       </c>
-      <c r="F9" s="71" t="s">
+      <c r="F9" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="70">
+      <c r="G9" s="34">
         <v>3</v>
       </c>
-      <c r="H9" s="70">
+      <c r="H9" s="34">
         <v>0.1</v>
       </c>
-      <c r="I9" s="72" t="s">
+      <c r="I9" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="77">
+      <c r="J9" s="41">
         <v>0.90639999999999998</v>
       </c>
-      <c r="K9" s="70">
+      <c r="K9" s="34">
         <v>0.82909999999999995</v>
       </c>
-      <c r="L9" s="70" t="s">
+      <c r="L9" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="M9" s="78" t="s">
+      <c r="M9" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="N9" s="60"/>
-      <c r="O9" s="61"/>
-      <c r="P9" s="62"/>
-      <c r="Q9" s="79">
+      <c r="N9" s="56"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="60"/>
+      <c r="Q9" s="43">
         <f t="shared" si="0"/>
         <v>7.7300000000000035E-2</v>
       </c>
     </row>
     <row r="10" spans="2:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="B10" s="52"/>
-      <c r="C10" s="40">
+      <c r="B10" s="46"/>
+      <c r="C10" s="30">
         <v>1E-4</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="5">
         <v>32</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="8">
         <v>10</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="5">
         <v>3</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="5">
         <v>0.1</v>
       </c>
-      <c r="I10" s="34" t="s">
+      <c r="I10" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="30">
+      <c r="J10" s="20">
         <v>0.90800000000000003</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="5">
         <v>0.82789999999999997</v>
       </c>
-      <c r="L10" s="11" t="s">
+      <c r="L10" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="M10" s="25" t="s">
+      <c r="M10" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="N10" s="60"/>
-      <c r="O10" s="61"/>
-      <c r="P10" s="62"/>
+      <c r="N10" s="56"/>
+      <c r="O10" s="58"/>
+      <c r="P10" s="60"/>
       <c r="Q10" s="1">
         <f t="shared" si="0"/>
         <v>8.010000000000006E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:17" s="79" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="B11" s="52"/>
-      <c r="C11" s="69">
+    <row r="11" spans="2:17" s="43" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B11" s="46"/>
+      <c r="C11" s="33">
         <v>1E-4</v>
       </c>
-      <c r="D11" s="70">
+      <c r="D11" s="34">
         <v>32</v>
       </c>
-      <c r="E11" s="73">
+      <c r="E11" s="37">
         <v>20</v>
       </c>
-      <c r="F11" s="75" t="s">
+      <c r="F11" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="70">
+      <c r="G11" s="34">
         <v>3</v>
       </c>
-      <c r="H11" s="70">
+      <c r="H11" s="34">
         <v>0.1</v>
       </c>
-      <c r="I11" s="72" t="s">
+      <c r="I11" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="77">
+      <c r="J11" s="41">
         <v>0.90610000000000002</v>
       </c>
-      <c r="K11" s="70">
+      <c r="K11" s="34">
         <v>0.82750000000000001</v>
       </c>
-      <c r="L11" s="70" t="s">
+      <c r="L11" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="M11" s="78" t="s">
+      <c r="M11" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="N11" s="60"/>
-      <c r="O11" s="61"/>
-      <c r="P11" s="62"/>
-      <c r="Q11" s="79">
+      <c r="N11" s="56"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="60"/>
+      <c r="Q11" s="43">
         <f t="shared" si="0"/>
         <v>7.8600000000000003E-2</v>
       </c>
     </row>
     <row r="12" spans="2:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="B12" s="52"/>
-      <c r="C12" s="5">
+      <c r="B12" s="46"/>
+      <c r="C12" s="30">
         <v>1E-4</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="5">
         <v>32</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="5">
         <v>15</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="5">
         <v>3</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="5">
         <v>0.1</v>
       </c>
-      <c r="I12" s="57" t="s">
+      <c r="I12" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="J12" s="23"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="80" t="s">
-        <v>67</v>
-      </c>
-      <c r="M12" s="26" t="s">
+      <c r="J12" s="20">
+        <v>0.91620000000000001</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0.82630000000000003</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="M12" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="N12" s="60"/>
-      <c r="O12" s="61"/>
-      <c r="P12" s="62"/>
+      <c r="N12" s="56"/>
+      <c r="O12" s="58"/>
+      <c r="P12" s="60"/>
       <c r="Q12" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.989999999999998E-2</v>
       </c>
     </row>
     <row r="13" spans="2:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="53"/>
-      <c r="C13" s="7">
+      <c r="B13" s="47"/>
+      <c r="C13" s="71">
         <v>1E-4</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="44">
         <v>32</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="44">
         <v>15</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="44">
         <v>3</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="44">
         <v>0.1</v>
       </c>
-      <c r="I13" s="58" t="s">
+      <c r="I13" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="J13" s="8"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="81" t="s">
-        <v>68</v>
-      </c>
-      <c r="M13" s="27" t="s">
+      <c r="J13" s="73">
+        <v>0.90690000000000004</v>
+      </c>
+      <c r="K13" s="44">
+        <v>0.82789999999999997</v>
+      </c>
+      <c r="L13" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" s="74" t="s">
         <v>62</v>
       </c>
-      <c r="N13" s="63"/>
-      <c r="O13" s="64"/>
-      <c r="P13" s="65"/>
+      <c r="N13" s="57"/>
+      <c r="O13" s="59"/>
+      <c r="P13" s="61"/>
       <c r="Q13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.900000000000007E-2</v>
       </c>
     </row>
     <row r="14" spans="2:17" ht="87" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="25">
         <v>1E-4</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="11">
         <v>32</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="11">
         <v>15</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="11">
         <v>3</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="11">
         <v>0.1</v>
       </c>
-      <c r="I14" s="36" t="s">
+      <c r="I14" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="31">
+      <c r="J14" s="21">
         <v>0.94259999999999999</v>
       </c>
-      <c r="K14" s="18">
+      <c r="K14" s="11">
         <v>0.84</v>
       </c>
-      <c r="L14" s="18" t="s">
+      <c r="L14" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="M14" s="28" t="s">
+      <c r="M14" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="N14" s="66" t="s">
+      <c r="N14" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="O14" s="67" t="s">
+      <c r="O14" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="P14" s="68" t="s">
+      <c r="P14" s="64" t="s">
         <v>24</v>
       </c>
       <c r="Q14" s="1">
@@ -1774,312 +1755,348 @@
         <v>0.10260000000000002</v>
       </c>
     </row>
-    <row r="15" spans="2:17" s="79" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="B15" s="52"/>
-      <c r="C15" s="76">
+    <row r="15" spans="2:17" s="43" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B15" s="46"/>
+      <c r="C15" s="40">
         <v>1E-3</v>
       </c>
-      <c r="D15" s="70">
+      <c r="D15" s="34">
         <v>32</v>
       </c>
-      <c r="E15" s="70">
+      <c r="E15" s="34">
         <v>15</v>
       </c>
-      <c r="F15" s="74" t="s">
+      <c r="F15" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="70">
+      <c r="G15" s="34">
         <v>3</v>
       </c>
-      <c r="H15" s="70">
+      <c r="H15" s="34">
         <v>0.1</v>
       </c>
-      <c r="I15" s="72" t="s">
+      <c r="I15" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="77">
+      <c r="J15" s="41">
         <v>0.87549999999999994</v>
       </c>
-      <c r="K15" s="70">
+      <c r="K15" s="34">
         <v>0.78869999999999996</v>
       </c>
-      <c r="L15" s="70" t="s">
+      <c r="L15" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="M15" s="78" t="s">
+      <c r="M15" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="N15" s="60"/>
-      <c r="O15" s="61"/>
-      <c r="P15" s="62"/>
-      <c r="Q15" s="79">
+      <c r="N15" s="56"/>
+      <c r="O15" s="58"/>
+      <c r="P15" s="60"/>
+      <c r="Q15" s="43">
         <f t="shared" si="0"/>
         <v>8.6799999999999988E-2</v>
       </c>
     </row>
     <row r="16" spans="2:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="B16" s="52"/>
-      <c r="C16" s="33">
+      <c r="B16" s="46"/>
+      <c r="C16" s="23">
         <v>0.01</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="5">
         <v>32</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="5">
         <v>15</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="5">
         <v>3</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="5">
         <v>0.1</v>
       </c>
-      <c r="I16" s="34" t="s">
+      <c r="I16" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="J16" s="30">
+      <c r="J16" s="20">
         <v>0.24590000000000001</v>
       </c>
-      <c r="K16" s="11">
+      <c r="K16" s="5">
         <v>0.2354</v>
       </c>
-      <c r="L16" s="11" t="s">
+      <c r="L16" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M16" s="25" t="s">
+      <c r="M16" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="N16" s="60"/>
-      <c r="O16" s="61"/>
-      <c r="P16" s="62"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="58"/>
+      <c r="P16" s="60"/>
       <c r="Q16" s="1">
         <f t="shared" si="0"/>
         <v>1.0500000000000009E-2</v>
       </c>
     </row>
     <row r="17" spans="2:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="B17" s="52"/>
-      <c r="C17" s="40">
+      <c r="B17" s="46"/>
+      <c r="C17" s="30">
         <v>1E-4</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="5">
         <v>32</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="5">
         <v>15</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="5">
         <v>3</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="5">
         <v>0.1</v>
       </c>
-      <c r="I17" s="34" t="s">
+      <c r="I17" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="J17" s="30">
+      <c r="J17" s="20">
         <v>0.94169999999999998</v>
       </c>
-      <c r="K17" s="11">
+      <c r="K17" s="5">
         <v>0.83819999999999995</v>
       </c>
-      <c r="L17" s="11" t="s">
+      <c r="L17" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="M17" s="25" t="s">
+      <c r="M17" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="N17" s="60"/>
-      <c r="O17" s="61"/>
-      <c r="P17" s="62"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="58"/>
+      <c r="P17" s="60"/>
       <c r="Q17" s="1">
         <f t="shared" si="0"/>
         <v>0.10350000000000004</v>
       </c>
     </row>
     <row r="18" spans="2:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="B18" s="52"/>
-      <c r="C18" s="40">
+      <c r="B18" s="46"/>
+      <c r="C18" s="30">
         <v>1E-4</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="5">
         <v>32</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="5">
         <v>15</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="5">
         <v>3</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="5">
         <v>0.1</v>
       </c>
-      <c r="I18" s="34" t="s">
+      <c r="I18" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="J18" s="30">
+      <c r="J18" s="20">
         <v>0.93310000000000004</v>
       </c>
-      <c r="K18" s="11">
+      <c r="K18" s="5">
         <v>0.84019999999999995</v>
       </c>
-      <c r="L18" s="11" t="s">
+      <c r="L18" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="M18" s="25" t="s">
+      <c r="M18" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="N18" s="60"/>
-      <c r="O18" s="61"/>
-      <c r="P18" s="62"/>
+      <c r="N18" s="56"/>
+      <c r="O18" s="58"/>
+      <c r="P18" s="60"/>
       <c r="Q18" s="1">
         <f t="shared" si="0"/>
         <v>9.2900000000000094E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:17" s="79" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="B19" s="52"/>
-      <c r="C19" s="69">
+    <row r="19" spans="2:17" s="43" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B19" s="46"/>
+      <c r="C19" s="33">
         <v>1E-4</v>
       </c>
-      <c r="D19" s="70">
+      <c r="D19" s="34">
         <v>32</v>
       </c>
-      <c r="E19" s="73">
+      <c r="E19" s="37">
         <v>10</v>
       </c>
-      <c r="F19" s="74" t="s">
+      <c r="F19" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="70">
+      <c r="G19" s="34">
         <v>3</v>
       </c>
-      <c r="H19" s="70">
+      <c r="H19" s="34">
         <v>0.1</v>
       </c>
-      <c r="I19" s="72" t="s">
+      <c r="I19" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="J19" s="77">
+      <c r="J19" s="41">
         <v>0.92849999999999999</v>
       </c>
-      <c r="K19" s="70">
+      <c r="K19" s="34">
         <v>0.84179999999999999</v>
       </c>
-      <c r="L19" s="70" t="s">
+      <c r="L19" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="M19" s="78" t="s">
+      <c r="M19" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="N19" s="60"/>
-      <c r="O19" s="61"/>
-      <c r="P19" s="62"/>
-      <c r="Q19" s="79">
+      <c r="N19" s="56"/>
+      <c r="O19" s="58"/>
+      <c r="P19" s="60"/>
+      <c r="Q19" s="43">
         <f t="shared" si="0"/>
         <v>8.6699999999999999E-2</v>
       </c>
     </row>
     <row r="20" spans="2:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="B20" s="52"/>
-      <c r="C20" s="5">
+      <c r="B20" s="46"/>
+      <c r="C20" s="30">
         <v>1E-4</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="5">
         <v>32</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="8">
         <v>20</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="5">
         <v>3</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="5">
         <v>0.1</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="J20" s="23"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="80" t="s">
+      <c r="J20" s="20">
+        <v>0.93310000000000004</v>
+      </c>
+      <c r="K20" s="5">
+        <v>0.84</v>
+      </c>
+      <c r="L20" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="M20" s="26" t="s">
+      <c r="M20" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="N20" s="60"/>
-      <c r="O20" s="61"/>
-      <c r="P20" s="62"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="58"/>
+      <c r="P20" s="60"/>
       <c r="Q20" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.3100000000000072E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B21" s="52"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="57" t="s">
+    <row r="21" spans="2:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="B21" s="46"/>
+      <c r="C21" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="D21" s="5">
+        <v>32</v>
+      </c>
+      <c r="E21" s="5">
+        <v>10</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="5">
+        <v>3</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="I21" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="J21" s="23"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2" t="s">
+      <c r="J21" s="20">
+        <v>0.94140000000000001</v>
+      </c>
+      <c r="K21" s="5">
+        <v>0.83579999999999999</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="M21" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="M21" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="N21" s="60"/>
-      <c r="O21" s="61"/>
-      <c r="P21" s="62"/>
+      <c r="N21" s="56"/>
+      <c r="O21" s="58"/>
+      <c r="P21" s="60"/>
       <c r="Q21" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.10560000000000003</v>
       </c>
     </row>
-    <row r="22" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="53"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="58" t="s">
+    <row r="22" spans="2:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="47"/>
+      <c r="C22" s="71">
+        <v>1E-4</v>
+      </c>
+      <c r="D22" s="44">
+        <v>32</v>
+      </c>
+      <c r="E22" s="44">
+        <v>10</v>
+      </c>
+      <c r="F22" s="72" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="44">
+        <v>3</v>
+      </c>
+      <c r="H22" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="I22" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="J22" s="8"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3" t="s">
+      <c r="J22" s="73">
+        <v>0.92889999999999995</v>
+      </c>
+      <c r="K22" s="44">
+        <v>0.83979999999999999</v>
+      </c>
+      <c r="L22" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="M22" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="M22" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="N22" s="63"/>
-      <c r="O22" s="64"/>
-      <c r="P22" s="65"/>
+      <c r="N22" s="57"/>
+      <c r="O22" s="59"/>
+      <c r="P22" s="61"/>
       <c r="Q22" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.9099999999999957E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>